<commit_message>
File in an xlsx file
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/Invalid.xlsx
+++ b/spec/fixtures/files/Invalid.xlsx
@@ -1,40 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulkristoff/dev/confirmation/spec/fixtures/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15960" windowHeight="16300"/>
+    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>Last Name</t>
   </si>
   <si>
-    <t>Cardinal Gibbons HS Group</t>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Teen Email</t>
+  </si>
+  <si>
+    <t>Parent Email Address(es)</t>
+  </si>
+  <si>
+    <t>Attending</t>
+  </si>
+  <si>
+    <t>program year</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
   <si>
     <t>Sophia</t>
@@ -46,12 +48,21 @@
     <t>vlagusta@aol.com</t>
   </si>
   <si>
+    <t>The Way</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
     <t>Ang</t>
   </si>
   <si>
     <t>joan3@nc.rr.com</t>
   </si>
   <si>
+    <t>Deferred</t>
+  </si>
+  <si>
     <t>Annunziata</t>
   </si>
   <si>
@@ -61,49 +72,62 @@
     <t>@nc.rr.com, rannunz</t>
   </si>
   <si>
+    <t>Abbreviated</t>
+  </si>
+  <si>
     <t>Bartos</t>
   </si>
   <si>
     <t>Britney</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Grade</t>
-  </si>
-  <si>
-    <t>Parent Email Address(es)</t>
-  </si>
-  <si>
-    <t>Teen Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="0" formatCode="General"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <u/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,18 +136,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -133,16 +151,38 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -161,105 +201,192 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+  <cellXfs count="22">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFAAAAAA"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="001FB714"/>
-      <rgbColor rgb="000000D4"/>
-      <rgbColor rgb="00FCF305"/>
-      <rgbColor rgb="00F20884"/>
-      <rgbColor rgb="0000ABEA"/>
-      <rgbColor rgb="00900000"/>
-      <rgbColor rgb="00006411"/>
-      <rgbColor rgb="00000090"/>
-      <rgbColor rgb="0090713A"/>
-      <rgbColor rgb="004600A5"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="0063AAFE"/>
-      <rgbColor rgb="00DD2D32"/>
-      <rgbColor rgb="00FFF58C"/>
-      <rgbColor rgb="004EE257"/>
-      <rgbColor rgb="006711FF"/>
-      <rgbColor rgb="00FEA746"/>
-      <rgbColor rgb="00865357"/>
-      <rgbColor rgb="00A2BD90"/>
-      <rgbColor rgb="0063AAFE"/>
-      <rgbColor rgb="00DD2D32"/>
-      <rgbColor rgb="00FFF58C"/>
-      <rgbColor rgb="004EE257"/>
-      <rgbColor rgb="006711FF"/>
-      <rgbColor rgb="00FEA746"/>
-      <rgbColor rgb="00865357"/>
-      <rgbColor rgb="00A2BD90"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffff0000"/>
+      <rgbColor rgb="ff00ff00"/>
+      <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffff00ff"/>
+      <rgbColor rgb="ff00ffff"/>
+      <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -301,14 +428,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office Theme">
       <a:majorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Helvetica"/>
-        <a:ea typeface="Helvetica"/>
-        <a:cs typeface="Helvetica"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office Theme">
@@ -385,7 +512,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -394,7 +521,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -403,9 +530,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -477,7 +604,7 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="38100" dist="23000" dir="5400000" rotWithShape="0">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
               <a:alpha val="35000"/>
             </a:srgbClr>
@@ -485,7 +612,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -504,19 +631,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Helvetica"/>
+            <a:ea typeface="Helvetica"/>
+            <a:cs typeface="Helvetica"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -534,7 +661,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -560,7 +687,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -586,7 +713,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -612,7 +739,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -638,7 +765,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -664,7 +791,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -690,7 +817,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -716,7 +843,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -742,7 +869,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -755,15 +882,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -778,15 +899,15 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="38100" dist="20000" dir="5400000" rotWithShape="0">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -805,7 +926,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -831,7 +952,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -857,7 +978,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -883,7 +1004,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -909,7 +1030,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -935,7 +1056,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -961,7 +1082,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -987,7 +1108,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1013,7 +1134,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1039,7 +1160,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1052,15 +1173,9 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1074,7 +1189,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1093,19 +1208,19 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Helvetica"/>
+            <a:ea typeface="Helvetica"/>
+            <a:cs typeface="Helvetica"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1123,7 +1238,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1149,7 +1264,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1175,7 +1290,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1201,7 +1316,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1227,7 +1342,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1253,7 +1368,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1279,7 +1394,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1305,7 +1420,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1331,7 +1446,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1344,322 +1459,388 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.3516" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="46.33203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="8.85156" style="1" customWidth="1"/>
+    <col min="5" max="5" width="46.3516" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="1" customWidth="1"/>
-    <col min="8" max="257" width="8.83203125" customWidth="1"/>
+    <col min="7" max="8" width="8.85156" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" ht="16.6" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" t="s" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="4">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="5">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="6"/>
+      <c r="B2" t="s" s="6">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s" s="6">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" t="s" s="6">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="G2" s="8">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s" s="6">
         <v>12</v>
       </c>
-      <c r="C1" s="8" t="s">
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" t="s" s="6">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" t="s" s="6">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="G3" s="8">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" t="s" s="6">
+        <v>11</v>
+      </c>
+      <c r="G4" s="8">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s" s="6">
         <v>15</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1"/>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3" t="s">
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s" s="10">
+        <v>19</v>
+      </c>
+      <c r="G5" s="8">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2"/>
+      <c r="H5" t="s" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="6"/>
+      <c r="F6" t="s" s="10">
+        <v>19</v>
+      </c>
+      <c r="G6" s="8">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="16"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="8.83203125" style="6" customWidth="1"/>
-    <col min="6" max="256" width="8.83203125" customWidth="1"/>
+    <col min="1" max="5" width="8.85156" style="20" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" ht="15" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="8.83203125" style="7" customWidth="1"/>
-    <col min="6" max="256" width="8.83203125" customWidth="1"/>
+    <col min="1" max="5" width="8.85156" style="21" customWidth="1"/>
+    <col min="6" max="16384" width="8.85156" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" ht="15" customHeight="1">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>